<commit_message>
File updates for revisions
</commit_message>
<xml_diff>
--- a/initial_values.xlsx
+++ b/initial_values.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iam\Box\Diversity-NSF\Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlichti\Box\Diversity-NSF\Lichti_et_al_Diversity_2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2DDF79-B65C-464D-B323-930990507201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38505" yWindow="-3390" windowWidth="38625" windowHeight="21225" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="density" sheetId="3" r:id="rId1"/>
@@ -28,12 +27,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
   <si>
     <t>species</t>
   </si>
@@ -80,9 +87,6 @@
     <t>age</t>
   </si>
   <si>
-    <t>rate</t>
-  </si>
-  <si>
     <t>resource</t>
   </si>
   <si>
@@ -145,11 +149,17 @@
   <si>
     <t>retrieve</t>
   </si>
+  <si>
+    <t>searchRate</t>
+  </si>
+  <si>
+    <t>relocationRate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,35 +470,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -496,13 +506,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -510,13 +520,13 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -524,35 +534,35 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -564,28 +574,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>5.9</v>
@@ -597,34 +607,44 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>18</v>
       </c>
       <c r="B3">
         <v>0.08</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -633,31 +653,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -669,21 +689,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -691,7 +711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -705,21 +725,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -730,7 +750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -747,47 +767,47 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -799,21 +819,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -824,7 +844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -835,9 +855,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>-1</v>
@@ -846,7 +866,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -863,21 +883,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -885,7 +905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>

</xml_diff>